<commit_message>
csv version added, lsr dxf deleted,
</commit_message>
<xml_diff>
--- a/STLs/STLprintSetting.xlsx
+++ b/STLs/STLprintSetting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000. Work\MCR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\000. Work\MCR\1. GitHub\sixi-2\STLs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03EC8BE-ABD2-42A8-ACBC-3015F15F1D16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89323911-76FE-437B-999C-1B4941726672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4561BAD2-1B40-4E4B-BBFD-B46A50BA8A05}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="137">
   <si>
     <t>[3D] - 1Aa-AnchorGearBox.stl</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>[3D] - 5Bd - outputDiskTOP.stl</t>
-  </si>
-  <si>
-    <t>[LSR] - MountingBoard 250mmx300mm.dxf</t>
   </si>
   <si>
     <t>File Name</t>
@@ -817,10 +814,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88E4D0A-E7E0-4956-B37F-2C616D474ABB}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,19 +831,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -857,13 +854,13 @@
         <v>0.2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1">
         <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -874,13 +871,13 @@
         <v>0.2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -891,13 +888,13 @@
         <v>0.2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1">
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -908,13 +905,13 @@
         <v>0.3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -925,13 +922,13 @@
         <v>0.3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -942,13 +939,13 @@
         <v>0.3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -959,50 +956,50 @@
         <v>0.3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="1">
         <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1">
         <v>0.2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1">
         <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1">
         <v>0.2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1">
         <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1013,13 +1010,13 @@
         <v>0.15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1">
         <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1030,13 +1027,13 @@
         <v>0.15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1">
         <v>100</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1047,13 +1044,13 @@
         <v>0.15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1">
         <v>100</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1064,13 +1061,13 @@
         <v>0.15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1">
         <v>100</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1081,13 +1078,13 @@
         <v>0.15</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1">
         <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1098,13 +1095,13 @@
         <v>0.15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1">
         <v>100</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1115,13 +1112,13 @@
         <v>0.15</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1">
         <v>100</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1132,13 +1129,13 @@
         <v>0.15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1">
         <v>100</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1149,693 +1146,693 @@
         <v>0.15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1">
         <v>100</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1">
         <v>0.15</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1">
         <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1">
         <v>0.15</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1">
         <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1">
         <v>0.15</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="1">
         <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1">
         <v>0.15</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="1">
         <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1">
         <v>0.15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="1">
         <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1">
         <v>0.15</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="1">
         <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1">
         <v>0.15</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="1">
         <v>100</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1">
         <v>0.15</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="1">
         <v>100</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1">
         <v>0.15</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="1">
         <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" s="1">
         <v>0.2</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="1">
         <v>20</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1">
         <v>0.2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="1">
         <v>20</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="1">
         <v>0.2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D31" s="1">
         <v>30</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32" s="1">
         <v>0.2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="1">
         <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1">
         <v>0.2</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="1">
         <v>20</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="1">
         <v>0.2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="1">
         <v>20</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1">
         <v>0.2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="1">
         <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B36" s="1">
         <v>0.15</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" s="1">
         <v>100</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="1">
         <v>0.15</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D37" s="1">
         <v>100</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="1">
         <v>0.15</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="1">
         <v>100</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="1">
         <v>0.15</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D39" s="1">
         <v>100</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="1">
         <v>0.15</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D40" s="1">
         <v>100</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" s="1">
         <v>0.2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D41" s="1">
         <v>20</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="1">
         <v>0.2</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D42" s="1">
         <v>20</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" s="1">
         <v>0.2</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" s="1">
         <v>20</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" s="1">
         <v>0.2</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D44" s="1">
         <v>20</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" s="1">
         <v>0.2</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D45" s="1">
         <v>30</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1">
         <v>0.2</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D46" s="1">
         <v>30</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="1">
         <v>0.2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D47" s="1">
         <v>30</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1">
         <v>0.15</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="1">
         <v>100</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B49" s="1">
         <v>0.15</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="1">
         <v>100</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" s="1">
         <v>0.15</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D50" s="1">
         <v>100</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B51" s="1">
         <v>0.15</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D51" s="1">
         <v>100</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B52" s="1">
         <v>0.15</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D52" s="1">
         <v>100</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B53" s="1">
         <v>0.2</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D53" s="1">
         <v>20</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B54" s="1">
         <v>0.15</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D54" s="1">
         <v>100</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" s="1">
         <v>0.2</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D55" s="1">
         <v>20</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B56" s="1">
         <v>0.15</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D56" s="1">
         <v>100</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B57" s="1">
         <v>0.15</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D57" s="1">
         <v>100</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B58" s="1">
         <v>0.15</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D58" s="1">
         <v>100</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B59" s="1">
         <v>0.15</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D59" s="1">
         <v>100</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1846,13 +1843,13 @@
         <v>0.2</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D60" s="1">
         <v>20</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1863,13 +1860,13 @@
         <v>0.2</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D61" s="1">
         <v>20</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1880,101 +1877,101 @@
         <v>0.2</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D62" s="1">
         <v>20</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B63" s="1">
         <v>0.2</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D63" s="1">
         <v>50</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B64" s="1">
         <v>0.2</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D64" s="1">
         <v>50</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B65" s="1">
         <v>0.2</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D65" s="1">
         <v>50</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B66" s="1">
         <v>0.2</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D66" s="1">
         <v>50</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B67" s="1">
         <v>0.2</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D67" s="1">
         <v>50</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1985,16 +1982,16 @@
         <v>0.2</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D68" s="1">
         <v>20</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2005,13 +2002,13 @@
         <v>0.2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D69" s="1">
         <v>20</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2022,13 +2019,13 @@
         <v>0.2</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D70" s="1">
         <v>20</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2039,13 +2036,13 @@
         <v>0.2</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D71" s="1">
         <v>30</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2056,13 +2053,13 @@
         <v>0.2</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D72" s="1">
         <v>30</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2073,13 +2070,13 @@
         <v>0.15</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D73" s="1">
         <v>100</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2090,13 +2087,13 @@
         <v>0.15</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D74" s="1">
         <v>100</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2107,13 +2104,13 @@
         <v>0.15</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D75" s="1">
         <v>100</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -2124,13 +2121,13 @@
         <v>0.15</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D76" s="1">
         <v>100</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -2141,13 +2138,13 @@
         <v>0.15</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D77" s="1">
         <v>100</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
@@ -2158,13 +2155,13 @@
         <v>0.2</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D78" s="1">
         <v>30</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -2175,13 +2172,13 @@
         <v>0.2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D79" s="1">
         <v>30</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2192,13 +2189,13 @@
         <v>0.2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D80" s="1">
         <v>30</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -2209,13 +2206,13 @@
         <v>0.2</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D81" s="1">
         <v>30</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -2226,13 +2223,13 @@
         <v>0.2</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D82" s="1">
         <v>30</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -2243,13 +2240,13 @@
         <v>0.2</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D83" s="1">
         <v>30</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -2260,13 +2257,13 @@
         <v>0.2</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D84" s="1">
         <v>30</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -2277,643 +2274,662 @@
         <v>0.2</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D85" s="1">
         <v>30</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B86" s="1">
         <v>0.15</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D86" s="1">
         <v>100</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B87" s="1">
         <v>0.2</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D87" s="1">
         <v>30</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B88" s="1">
         <v>0.2</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D88" s="1">
         <v>30</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B89" s="1">
         <v>0.2</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D89" s="1">
         <v>20</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B90" s="1">
         <v>0.2</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D90" s="1">
         <v>20</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B91" s="1">
         <v>0.2</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D91" s="1">
         <v>30</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B92" s="1">
         <v>0.2</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D92" s="1">
         <v>30</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B93" s="1">
         <v>0.2</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D93" s="1">
         <v>20</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B94" s="1">
         <v>0.2</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D94" s="1">
         <v>30</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B95" s="1">
         <v>0.15</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D95" s="1">
         <v>100</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B96" s="1">
         <v>0.15</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D96" s="1">
         <v>100</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B97" s="1">
         <v>0.15</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D97" s="1">
         <v>100</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B98" s="1">
         <v>0.2</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D98" s="1">
         <v>30</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B99" s="1">
         <v>0.2</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D99" s="1">
         <v>30</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B100" s="1">
         <v>0.2</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D100" s="1">
         <v>30</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B101" s="1">
         <v>0.15</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D101" s="1">
         <v>100</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B102" s="1">
         <v>0.15</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D102" s="1">
         <v>100</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B103" s="1">
         <v>0.15</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D103" s="1">
         <v>100</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B104" s="1">
         <v>0.15</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D104" s="1">
         <v>100</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B105" s="1">
         <v>0.2</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D105" s="1">
         <v>30</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B106" s="1">
         <v>0.15</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D106" s="1">
         <v>100</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B107" s="1">
         <v>0.15</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D107" s="1">
         <v>100</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B108" s="1">
         <v>0.2</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D108" s="1">
         <v>30</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B109" s="1">
         <v>0.2</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D109" s="1">
         <v>30</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B110" s="1">
         <v>0.15</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D110" s="1">
         <v>100</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B111" s="1">
         <v>0.15</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D111" s="1">
         <v>100</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B112" s="1">
         <v>0.15</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D112" s="1">
         <v>100</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B113" s="1">
         <v>0.15</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D113" s="1">
         <v>100</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B114" s="1">
         <v>0.2</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D114" s="1">
         <v>30</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B115" s="1">
         <v>0.2</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D115" s="1">
         <v>30</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B116" s="1">
         <v>0.2</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D116" s="1">
         <v>20</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B117" s="1">
         <v>0.2</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D117" s="1">
         <v>20</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B118" s="1">
         <v>0.2</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D118" s="1">
         <v>20</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B119" s="1">
         <v>0.2</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D119" s="1">
         <v>20</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B120" s="1">
         <v>0.2</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D120" s="1">
         <v>20</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B121" s="1">
         <v>0.2</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D121" s="1">
         <v>20</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="B122" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D122" s="1">
+        <v>20</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>37</v>
+        <v>135</v>
+      </c>
+      <c r="B123" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D123" s="1">
+        <v>20</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>